<commit_message>
added prerequiste for revoking license
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Billing/manual_discount_test_data.xlsx
+++ b/TestData/Web_POS/Billing/manual_discount_test_data.xlsx
@@ -75,13 +75,13 @@
     <t>TC_01</t>
   </si>
   <si>
-    <t>3072406240Vp</t>
+    <t>307260624WoJ</t>
   </si>
   <si>
     <t>zwshashank.agrawal@teampureplay.com</t>
   </si>
   <si>
-    <t>NewIndex</t>
+    <t>usertwo_p1</t>
   </si>
   <si>
     <t>Index9QA</t>
@@ -120,6 +120,9 @@
     <t>list : Percentage_Item</t>
   </si>
   <si>
+    <t>Percentage : 10</t>
+  </si>
+  <si>
     <t>TC_04</t>
   </si>
   <si>
@@ -195,9 +198,6 @@
     <t>Custom_Discount_Percentage : 10</t>
   </si>
   <si>
-    <t>Percentage : 10</t>
-  </si>
-  <si>
     <t>TC_16</t>
   </si>
   <si>
@@ -228,15 +228,36 @@
     <t>TC_25</t>
   </si>
   <si>
+    <t>307260624ut0</t>
+  </si>
+  <si>
+    <t>usertwo_p2</t>
+  </si>
+  <si>
     <t>TC_26</t>
   </si>
   <si>
+    <t>userone_p1</t>
+  </si>
+  <si>
     <t>TC_27</t>
   </si>
   <si>
+    <t>307260624PTe</t>
+  </si>
+  <si>
+    <t>userone_p4</t>
+  </si>
+  <si>
     <t>TC_28</t>
   </si>
   <si>
+    <t>307260624uOm</t>
+  </si>
+  <si>
+    <t>userone_p5</t>
+  </si>
+  <si>
     <t>TC_29</t>
   </si>
   <si>
@@ -264,15 +285,30 @@
     <t>TC_33</t>
   </si>
   <si>
+    <t>userone_p2</t>
+  </si>
+  <si>
     <t>TC_34</t>
   </si>
   <si>
     <t>TC_35</t>
   </si>
   <si>
+    <t>307260624SF2</t>
+  </si>
+  <si>
+    <t>userone_p6</t>
+  </si>
+  <si>
     <t>TC_36</t>
   </si>
   <si>
+    <t>307260624cuS</t>
+  </si>
+  <si>
+    <t>userone_p7</t>
+  </si>
+  <si>
     <t>TC_37</t>
   </si>
   <si>
@@ -316,6 +352,12 @@
   </si>
   <si>
     <t>TC_45</t>
+  </si>
+  <si>
+    <t>3072606245nJ</t>
+  </si>
+  <si>
+    <t>userone_p3</t>
   </si>
   <si>
     <t>TC_46</t>
@@ -613,8 +655,8 @@
     <outlinePr summaryRight="0" summaryBelow="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="K25">
-      <selection activeCell="S37" sqref="S37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
@@ -858,12 +900,12 @@
         <v>32</v>
       </c>
       <c r="Q4" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>18</v>
@@ -908,15 +950,15 @@
         <v>26</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Q5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" ht="26.25" customHeight="1">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>18</v>
@@ -961,7 +1003,7 @@
         <v>26</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="Q6" t="s">
         <v>28</v>
@@ -969,7 +1011,7 @@
     </row>
     <row r="7" ht="30" customHeight="1">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>18</v>
@@ -1014,15 +1056,15 @@
         <v>26</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Q7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" ht="31.5" customHeight="1">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>18</v>
@@ -1067,7 +1109,7 @@
         <v>26</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Q8" t="s">
         <v>28</v>
@@ -1075,7 +1117,7 @@
     </row>
     <row r="9" ht="32.25" customHeight="1">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>18</v>
@@ -1120,15 +1162,15 @@
         <v>26</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Q9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" ht="28.5" customHeight="1">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>18</v>
@@ -1173,7 +1215,7 @@
         <v>26</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="Q10" t="s">
         <v>28</v>
@@ -1181,7 +1223,7 @@
     </row>
     <row r="11" ht="14.25">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>18</v>
@@ -1226,7 +1268,7 @@
         <v>26</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="Q11" t="s">
         <v>28</v>
@@ -1234,7 +1276,7 @@
     </row>
     <row r="12" ht="14.25">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>18</v>
@@ -1279,7 +1321,7 @@
         <v>26</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Q12" t="s">
         <v>28</v>
@@ -1287,7 +1329,7 @@
     </row>
     <row r="13" ht="14.25">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>18</v>
@@ -1332,7 +1374,7 @@
         <v>26</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="Q13" t="s">
         <v>28</v>
@@ -1340,7 +1382,7 @@
     </row>
     <row r="14" ht="14.25">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>18</v>
@@ -1385,7 +1427,7 @@
         <v>26</v>
       </c>
       <c r="P14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="Q14" t="s">
         <v>28</v>
@@ -1393,7 +1435,7 @@
     </row>
     <row r="15" ht="14.25">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>18</v>
@@ -1438,7 +1480,7 @@
         <v>26</v>
       </c>
       <c r="P15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="Q15" t="s">
         <v>28</v>
@@ -1446,7 +1488,7 @@
     </row>
     <row r="16" ht="14.25">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>18</v>
@@ -1491,10 +1533,10 @@
         <v>26</v>
       </c>
       <c r="P16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="Q16" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" ht="14.25">
@@ -1544,7 +1586,7 @@
         <v>26</v>
       </c>
       <c r="P17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="Q17" t="s">
         <v>28</v>
@@ -1597,7 +1639,7 @@
         <v>26</v>
       </c>
       <c r="P18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="Q18" t="s">
         <v>28</v>
@@ -1650,10 +1692,10 @@
         <v>26</v>
       </c>
       <c r="P19" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="Q19" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" ht="14.25">
@@ -1862,10 +1904,10 @@
         <v>26</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Q23" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" ht="14.25">
@@ -1915,7 +1957,7 @@
         <v>26</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="Q24" t="s">
         <v>28</v>
@@ -1972,10 +2014,10 @@
         <v>26</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Q25" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" ht="14.25">
@@ -1983,7 +2025,7 @@
         <v>68</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>19</v>
@@ -1992,7 +2034,7 @@
         <v>123456</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="F26" s="2">
         <v>123456</v>
@@ -2033,7 +2075,7 @@
     </row>
     <row r="27" ht="14.25">
       <c r="A27" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>18</v>
@@ -2045,7 +2087,7 @@
         <v>123456</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="F27" s="2">
         <v>123456</v>
@@ -2086,10 +2128,10 @@
     </row>
     <row r="28" ht="14.25">
       <c r="A28" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>19</v>
@@ -2098,7 +2140,7 @@
         <v>123456</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>20</v>
+        <v>75</v>
       </c>
       <c r="F28" s="2">
         <v>123456</v>
@@ -2139,10 +2181,10 @@
     </row>
     <row r="29" ht="14.25">
       <c r="A29" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>19</v>
@@ -2151,7 +2193,7 @@
         <v>123456</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="F29" s="2">
         <v>123456</v>
@@ -2196,10 +2238,10 @@
     </row>
     <row r="30" ht="14.25">
       <c r="A30" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>19</v>
@@ -2208,7 +2250,7 @@
         <v>123456</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>20</v>
+        <v>75</v>
       </c>
       <c r="F30" s="2">
         <v>123456</v>
@@ -2253,10 +2295,10 @@
     </row>
     <row r="31" ht="14.25">
       <c r="A31" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>19</v>
@@ -2265,7 +2307,7 @@
         <v>123456</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="F31" s="2">
         <v>123456</v>
@@ -2310,11 +2352,11 @@
     </row>
     <row r="32" ht="14.25">
       <c r="A32" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="C32" s="2" t="s">
         <v>19</v>
       </c>
@@ -2322,7 +2364,7 @@
         <v>123456</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>20</v>
+        <v>75</v>
       </c>
       <c r="F32" s="2">
         <v>123456</v>
@@ -2355,10 +2397,10 @@
         <v>26</v>
       </c>
       <c r="P32" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="Q32" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="T32" s="4"/>
       <c r="U32" s="4"/>
@@ -2367,10 +2409,10 @@
     </row>
     <row r="33" ht="14.25">
       <c r="A33" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>19</v>
@@ -2379,7 +2421,7 @@
         <v>123456</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>20</v>
+        <v>75</v>
       </c>
       <c r="F33" s="2">
         <v>123456</v>
@@ -2412,10 +2454,10 @@
         <v>26</v>
       </c>
       <c r="P33" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="Q33" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="T33" s="4"/>
       <c r="U33" s="4"/>
@@ -2424,10 +2466,10 @@
     </row>
     <row r="34" ht="14.25">
       <c r="A34" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>19</v>
@@ -2436,7 +2478,7 @@
         <v>123456</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>20</v>
+        <v>88</v>
       </c>
       <c r="F34" s="2">
         <v>123456</v>
@@ -2478,7 +2520,7 @@
     </row>
     <row r="35" ht="14.25">
       <c r="A35" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>18</v>
@@ -2532,10 +2574,10 @@
     </row>
     <row r="36" ht="14.25">
       <c r="A36" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>18</v>
+        <v>91</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>19</v>
@@ -2544,7 +2586,7 @@
         <v>123456</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="F36" s="2">
         <v>123456</v>
@@ -2588,10 +2630,10 @@
     </row>
     <row r="37" ht="14.25">
       <c r="A37" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>18</v>
+        <v>94</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>19</v>
@@ -2600,7 +2642,7 @@
         <v>123456</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>20</v>
+        <v>95</v>
       </c>
       <c r="F37" s="2">
         <v>123456</v>
@@ -2641,10 +2683,10 @@
     </row>
     <row r="38" ht="14.25">
       <c r="A38" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>18</v>
+        <v>91</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>19</v>
@@ -2653,7 +2695,7 @@
         <v>123456</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="F38" s="2">
         <v>123456</v>
@@ -2698,10 +2740,10 @@
     </row>
     <row r="39" ht="14.25">
       <c r="A39" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>18</v>
+        <v>94</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>19</v>
@@ -2710,7 +2752,7 @@
         <v>123456</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>20</v>
+        <v>95</v>
       </c>
       <c r="F39" s="2">
         <v>123456</v>
@@ -2751,10 +2793,10 @@
     </row>
     <row r="40" ht="14.25">
       <c r="A40" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>18</v>
+        <v>91</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>19</v>
@@ -2763,7 +2805,7 @@
         <v>123456</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="F40" s="2">
         <v>123456</v>
@@ -2796,18 +2838,18 @@
         <v>26</v>
       </c>
       <c r="P40" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="Q40" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
     </row>
     <row r="41" ht="14.25">
       <c r="A41" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>18</v>
+        <v>91</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>19</v>
@@ -2816,7 +2858,7 @@
         <v>123456</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="F41" s="2">
         <v>123456</v>
@@ -2849,15 +2891,15 @@
         <v>26</v>
       </c>
       <c r="P41" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="Q41" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
     </row>
     <row r="42" ht="14.25">
       <c r="A42" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>18</v>
@@ -2902,15 +2944,15 @@
         <v>26</v>
       </c>
       <c r="P42" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="Q42" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" ht="14.25">
       <c r="A43" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>18</v>
@@ -2955,15 +2997,15 @@
         <v>26</v>
       </c>
       <c r="P43" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="Q43" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
     </row>
     <row r="44" ht="14.25">
       <c r="A44" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>18</v>
@@ -3016,7 +3058,7 @@
     </row>
     <row r="45" ht="14.25">
       <c r="A45" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>18</v>
@@ -3069,10 +3111,10 @@
     </row>
     <row r="46" ht="14.25">
       <c r="A46" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>18</v>
+        <v>111</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>19</v>
@@ -3081,7 +3123,7 @@
         <v>123456</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>20</v>
+        <v>112</v>
       </c>
       <c r="F46" s="2">
         <v>123456</v>
@@ -3122,10 +3164,10 @@
     </row>
     <row r="47" ht="14.25">
       <c r="A47" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>18</v>
+        <v>111</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>19</v>
@@ -3134,7 +3176,7 @@
         <v>123456</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>20</v>
+        <v>112</v>
       </c>
       <c r="F47" s="2">
         <v>123456</v>

</xml_diff>